<commit_message>
committed new code on 06/19 with test data details-Pavan
</commit_message>
<xml_diff>
--- a/Testdata/Testdata.xlsx
+++ b/Testdata/Testdata.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="CommonTestdata" sheetId="1" r:id="rId1"/>
-    <sheet name="Headers" sheetId="2" r:id="rId2"/>
+    <sheet name="Fieldinfo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Sno</t>
   </si>
@@ -40,33 +40,15 @@
     <t>QA</t>
   </si>
   <si>
-    <t>user01</t>
-  </si>
-  <si>
-    <t>pass1234</t>
-  </si>
-  <si>
     <t>Tc_Name</t>
   </si>
   <si>
     <t>Iteration</t>
   </si>
   <si>
-    <t>From_Date</t>
-  </si>
-  <si>
-    <t>To_Date</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>http://automationpractice.com/index.php</t>
   </si>
   <si>
-    <t>Headers</t>
-  </si>
-  <si>
     <t>TC_01_Verify_Forgotpwd_link_is_available</t>
   </si>
   <si>
@@ -74,6 +56,63 @@
   </si>
   <si>
     <t>Please enter the email address you used to register.</t>
+  </si>
+  <si>
+    <t>Text1</t>
+  </si>
+  <si>
+    <t>Email address</t>
+  </si>
+  <si>
+    <t>Authentication</t>
+  </si>
+  <si>
+    <t>Text2</t>
+  </si>
+  <si>
+    <t>Header1</t>
+  </si>
+  <si>
+    <t>Forgot your password?</t>
+  </si>
+  <si>
+    <t>Header2</t>
+  </si>
+  <si>
+    <t>Error1</t>
+  </si>
+  <si>
+    <t>There is 1 error</t>
+  </si>
+  <si>
+    <t>Error2</t>
+  </si>
+  <si>
+    <t>Invalid email address.</t>
+  </si>
+  <si>
+    <t>Rtrpwd</t>
+  </si>
+  <si>
+    <t>Retrieve Password</t>
+  </si>
+  <si>
+    <t>Bck2Login</t>
+  </si>
+  <si>
+    <t>Back to Login</t>
+  </si>
+  <si>
+    <t>Forgotlink</t>
+  </si>
+  <si>
+    <t>Authlink</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>abcd</t>
   </si>
 </sst>
 </file>
@@ -139,13 +178,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -430,7 +470,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -465,13 +505,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -553,105 +587,204 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:13">
       <c r="A1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
+      <c r="D2" s="4"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
+      <c r="D6" s="4"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
+      <c r="D7" s="4"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
+      <c r="D8" s="4"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>